<commit_message>
Cambios Devoluciones y control stock Nutri
</commit_message>
<xml_diff>
--- a/Engine V2/Ruta4.xlsx
+++ b/Engine V2/Ruta4.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="ErroresCarga" sheetId="1" r:id="rId1"/>
+    <sheet name="Formato" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -32,22 +32,22 @@
     <t>Errores</t>
   </si>
   <si>
-    <t>60000312</t>
+    <t>60000050</t>
   </si>
   <si>
-    <t>Leche Polietileno Entera 400ml</t>
+    <t>Leche Semidescremada Tetrafino 900ml</t>
   </si>
   <si>
-    <t>Leonardo Ortiz</t>
+    <t>Christopher Hablich</t>
   </si>
   <si>
-    <t>1717576878</t>
+    <t>0921821419</t>
   </si>
   <si>
-    <t>10</t>
+    <t>120</t>
   </si>
   <si>
-    <t>El producto no se encuentra registrado</t>
+    <t>El distribuidor no se encuentra registrado-No tiene suficiente STOCK. Cantidad actual: 42,0000</t>
   </si>
 </sst>
 </file>

</xml_diff>